<commit_message>
Added the functional test case of active booking consumer
</commit_message>
<xml_diff>
--- a/credentials/credentials.xlsx
+++ b/credentials/credentials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayakaushik\Documents\Product_Week\credentials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdadheech\Parking-Slot-Booking\credentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A2F96F-F121-4F01-82EA-ED161C345CE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB636BF2-42D2-45D6-BAC5-2CDB3B535D6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>email</t>
   </si>
@@ -40,6 +40,36 @@
   </si>
   <si>
     <t>consumer2@gmail.com</t>
+  </si>
+  <si>
+    <t>PaymentEmail</t>
+  </si>
+  <si>
+    <t>PaymentCardNo</t>
+  </si>
+  <si>
+    <t>PaymentMMYY</t>
+  </si>
+  <si>
+    <t>Paymentcvv</t>
+  </si>
+  <si>
+    <t>PaymentNameOnCard</t>
+  </si>
+  <si>
+    <t>PaymentCountry</t>
+  </si>
+  <si>
+    <t>Mahesh</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Extended_time</t>
+  </si>
+  <si>
+    <t>Extended date</t>
   </si>
 </sst>
 </file>
@@ -84,9 +114,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -368,19 +400,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.36328125" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,7 +426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -396,12 +434,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3">
+        <v>4242424242424240</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44585</v>
+      </c>
+      <c r="D9">
+        <v>234</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>44677</v>
       </c>
     </row>
   </sheetData>
@@ -410,7 +498,9 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{8D76F59E-5CC3-407E-A893-E81D1F8445E7}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{4A4E2253-3C31-4588-8D5C-6E8F8D243E92}"/>
     <hyperlink ref="B3" r:id="rId4" xr:uid="{8402AC29-5071-4A9D-84F1-E8EF3BF30201}"/>
+    <hyperlink ref="A9" r:id="rId5" xr:uid="{4CD0CC4A-8D4E-4B9D-A838-06671FCB4E0D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Extent reports and screenshot listeners
</commit_message>
<xml_diff>
--- a/credentials/credentials.xlsx
+++ b/credentials/credentials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihirsharma\Parking-Slot-Booking\credentials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayakaushik\Documents\Product_Week\credentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AE5AB7-85CF-4407-9A70-E3E6F398BBD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659ECFDD-539E-4797-9D6A-D5CAF6F9A399}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>email</t>
   </si>
@@ -34,9 +34,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>provider1@gmail.com</t>
-  </si>
-  <si>
     <t>password@123</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>location</t>
   </si>
   <si>
-    <t>The Great Indian Place</t>
-  </si>
-  <si>
     <t>entry date</t>
   </si>
   <si>
@@ -74,13 +68,49 @@
   </si>
   <si>
     <t>exit time</t>
+  </si>
+  <si>
+    <t>provider2@gmail.com</t>
+  </si>
+  <si>
+    <t>consumer20</t>
+  </si>
+  <si>
+    <t>consumer20@gmail.com</t>
+  </si>
+  <si>
+    <t>provider121@gmail.com</t>
+  </si>
+  <si>
+    <t>Vehicle Number</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>UP137788</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>provider121</t>
+  </si>
+  <si>
+    <t>provider909@gmail.com</t>
+  </si>
+  <si>
+    <t>The Great India Place</t>
+  </si>
+  <si>
+    <t>provider909</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +122,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,11 +163,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -404,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -431,69 +477,124 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2">
-        <v>44677</v>
-      </c>
-      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3">
+        <v>4262022</v>
+      </c>
+      <c r="H2" s="4">
         <v>0.625</v>
       </c>
-      <c r="I2" s="2">
-        <v>44679</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="I2" s="3">
+        <v>4282022</v>
+      </c>
+      <c r="J2" s="4">
         <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -501,8 +602,12 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{8D76F59E-5CC3-407E-A893-E81D1F8445E7}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{4A4E2253-3C31-4588-8D5C-6E8F8D243E92}"/>
     <hyperlink ref="B3" r:id="rId4" xr:uid="{8402AC29-5071-4A9D-84F1-E8EF3BF30201}"/>
-    <hyperlink ref="D2" r:id="rId5" xr:uid="{629B4B5E-F2C5-4FE4-A6FF-A40FCA0BB765}"/>
-    <hyperlink ref="E2" r:id="rId6" xr:uid="{6BB4F019-A6F1-47A9-9180-A12D2FAE4696}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{E0FB1A4D-200C-4124-8E79-F2CAC4068177}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{64ACD86F-A88F-48A9-B95E-D12A2F36B82E}"/>
+    <hyperlink ref="A4" r:id="rId7" display="mailto:provider121@gmail.com" xr:uid="{75794F71-B765-4359-8803-EF237DE33D79}"/>
+    <hyperlink ref="B4" r:id="rId8" display="mailto:password@123" xr:uid="{2EB8B6D5-B923-4BBD-A270-FBC5A20FCD1E}"/>
+    <hyperlink ref="D2" r:id="rId9" display="mailto:provider909@gmail.com" xr:uid="{4F452A66-52A2-40F6-BF75-BFBE834F4125}"/>
+    <hyperlink ref="E2" r:id="rId10" display="mailto:password@123" xr:uid="{98375937-799A-4439-8EF6-B733FC702EE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -525,24 +630,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>